<commit_message>
operative situation reports report export & weather summary
</commit_message>
<xml_diff>
--- a/aho.xlsx
+++ b/aho.xlsx
@@ -5,13 +5,13 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Заявки АХО" sheetId="1" r:id="rId1"/>
+    <sheet name="Оперативная обстановка" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>#</t>
   </si>
@@ -19,7 +19,7 @@
     <t>Дата подачи</t>
   </si>
   <si>
-    <t>Заявитель</t>
+    <t>Инициатор / Заявитель</t>
   </si>
   <si>
     <t>Срок исполн.</t>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Статус</t>
+  </si>
+  <si>
+    <t>Телефон</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -108,9 +111,10 @@
     <col min="6" max="6" width="35" customWidth="1"/>
     <col min="7" max="7" width="40" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20" customHeight="1">
+    <row r="1" spans="1:9" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -135,6 +139,9 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>